<commit_message>
Re-plotted naive since it changed
</commit_message>
<xml_diff>
--- a/Assignment1_Workbook.xlsx
+++ b/Assignment1_Workbook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5960" yWindow="-18220" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,18 +27,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>n</t>
   </si>
   <si>
-    <t>Brute Force (s)</t>
+    <t>Brute Force</t>
   </si>
   <si>
-    <t>Naive D&amp;C (s)</t>
+    <t>Enhanced D&amp;C</t>
   </si>
   <si>
-    <t>Enhanced D&amp;C (s)</t>
+    <t>time (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naive D&amp;C </t>
   </si>
 </sst>
 </file>
@@ -77,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -86,6 +89,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -309,16 +315,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.00126261998957488</c:v>
+                  <c:v>0.00152883199916686</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0132787530019413</c:v>
+                  <c:v>0.0229527979972772</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.147379150992492</c:v>
+                  <c:v>0.374633359009749</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.61736529300105</c:v>
+                  <c:v>5.41545580299862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,16 +1222,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1510,19 +1516,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E3:H7"/>
+  <dimension ref="E2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
     <row r="3" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E3" s="2" t="s">
         <v>0</v>
@@ -1531,10 +1544,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="5:8" x14ac:dyDescent="0.2">
@@ -1544,8 +1557,8 @@
       <c r="F4" s="3">
         <v>7.7089200058253404E-3</v>
       </c>
-      <c r="G4">
-        <v>1.2626199895748799E-3</v>
+      <c r="G4" s="2">
+        <v>1.52883199916686E-3</v>
       </c>
     </row>
     <row r="5" spans="5:8" x14ac:dyDescent="0.2">
@@ -1555,8 +1568,8 @@
       <c r="F5" s="2">
         <v>0.785602477000793</v>
       </c>
-      <c r="G5">
-        <v>1.32787530019413E-2</v>
+      <c r="G5" s="2">
+        <v>2.2952797997277199E-2</v>
       </c>
     </row>
     <row r="6" spans="5:8" x14ac:dyDescent="0.2">
@@ -1566,19 +1579,22 @@
       <c r="F6" s="2">
         <v>77.323869009996997</v>
       </c>
-      <c r="G6">
-        <v>0.14737915099249199</v>
+      <c r="G6" s="2">
+        <v>0.37463335900974898</v>
       </c>
     </row>
     <row r="7" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E7" s="1">
         <v>100000</v>
       </c>
-      <c r="G7">
-        <v>1.61736529300105</v>
+      <c r="G7" s="2">
+        <v>5.4154558029986202</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
took 100k input timing for brute_force
</commit_message>
<xml_diff>
--- a/Assignment1_Workbook.xlsx
+++ b/Assignment1_Workbook.xlsx
@@ -302,7 +302,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -651,11 +651,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="54209480"/>
-        <c:axId val="4369476"/>
+        <c:axId val="69368416"/>
+        <c:axId val="4393898"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54209480"/>
+        <c:axId val="69368416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -731,12 +731,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4369476"/>
+        <c:crossAx val="4393898"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4369476"/>
+        <c:axId val="4393898"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +812,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54209480"/>
+        <c:crossAx val="69368416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -907,7 +907,7 @@
   <dimension ref="E1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -990,7 +990,9 @@
       <c r="E7" s="9" t="n">
         <v>100000</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="10" t="n">
+        <v>4274.648500398</v>
+      </c>
       <c r="G7" s="10" t="n">
         <v>6.95278498199968</v>
       </c>

</xml_diff>